<commit_message>
misc tool to resave xlsx files
</commit_message>
<xml_diff>
--- a/raw_data/9.15 Cell Growth/9-15 cell density.xlsx
+++ b/raw_data/9.15 Cell Growth/9-15 cell density.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/mobile/Containers/Data/Application/039FBA4F-CB45-4E06-9DF7-161818EEE98A/Library/Application Support/Drafts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox (GaTech)\Lab files\code\Impedance_fit\raw_data\9.15 Cell Growth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE2DA00B-2883-154F-84B6-CBADB9656F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C6FA69-B298-4F70-A136-C1358C01B402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,9 +405,9 @@
       <selection activeCell="L26" sqref="L26:L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44089</v>
       </c>
@@ -429,17 +429,17 @@
         <v>221000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="3">
         <v>339000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="3">
         <v>331000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>0.66666666666666663</v>
       </c>
@@ -447,17 +447,17 @@
         <v>686000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" s="3">
         <v>505000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" s="3">
         <v>328000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>0.79166666666666663</v>
       </c>
@@ -465,17 +465,17 @@
         <v>336000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C9" s="3">
         <v>383000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" s="3">
         <v>456000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44090</v>
       </c>
@@ -486,17 +486,17 @@
         <v>366000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C12" s="3">
         <v>393000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="3">
         <v>598000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <v>0.5</v>
       </c>
@@ -504,17 +504,17 @@
         <v>475000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" s="3">
         <v>530000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="3">
         <v>574000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>0.625</v>
       </c>
@@ -522,17 +522,17 @@
         <v>536000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C18" s="3">
         <v>538000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C19" s="3">
         <v>495000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>0.75</v>
       </c>
@@ -540,17 +540,17 @@
         <v>1260000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C21" s="3">
         <v>396000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C22" s="3">
         <v>555000</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>0.875</v>
       </c>
@@ -558,17 +558,17 @@
         <v>852000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C24" s="3">
         <v>831000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C25" s="3">
         <v>1170000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44091</v>
       </c>
@@ -579,12 +579,12 @@
         <v>956000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C27" s="3">
         <v>1490000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C28" s="3">
         <v>986000</v>
       </c>

</xml_diff>